<commit_message>
Clean up and Page creator
</commit_message>
<xml_diff>
--- a/_Tests/Tableau.xlsx
+++ b/_Tests/Tableau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etienne\Desktop\DeepCodeur v2\DeepCodeur\_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5CB68D-DF79-43EF-9FAE-24AF3363EBCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1401DA72-BD07-457E-964C-69D7480E987A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="452">
   <si>
     <t>Balise html</t>
   </si>
@@ -1547,6 +1547,9 @@
   <si>
     <t>sous fenetre,
 implemente</t>
+  </si>
+  <si>
+    <t>paragraphe</t>
   </si>
 </sst>
 </file>
@@ -3708,10 +3711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F397223-A21C-45D8-B597-6C8BF678C705}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4007,131 +4010,139 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>398</v>
+        <v>451</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>399</v>
+        <v>451</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>411</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>412</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>